<commit_message>
dati gm,R0,lambda conclusivi (curva dei Pmos per r0 non corretta, i gm sembrano ok)
</commit_message>
<xml_diff>
--- a/MicroB/testmat/DATI_correnti_gm.xlsx
+++ b/MicroB/testmat/DATI_correnti_gm.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github-Repo\MicroElectronics\MicroB\testmat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19CFCA7-B66A-4C10-9D6D-FFE132F07483}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA799C4C-C3E3-4763-9C38-56CB5E3C424F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4275" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
+    <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -377,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,90 +397,832 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>0.80000001192092896</v>
       </c>
       <c r="B2">
-        <v>-1.1790372280925943E-12</v>
+        <v>-8.1037612601267406E-13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1.2999999523162842</v>
+        <v>0.89999997615814209</v>
       </c>
       <c r="B3">
-        <v>-1.2618587286183924E-9</v>
+        <v>-9.1798259532066551E-13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1.6000000238418579</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>-5.7786155593930744E-7</v>
+        <v>-1.1790372280925943E-12</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1.8999999761581421</v>
+        <v>1.1000000238418579</v>
       </c>
       <c r="B5">
-        <v>-4.4340358726913109E-6</v>
+        <v>-4.6577945493619932E-12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2.2000000476837158</v>
+        <v>1.2000000476837158</v>
       </c>
       <c r="B6">
-        <v>-1.156148937297985E-5</v>
+        <v>-7.2908491743906012E-11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2.5</v>
+        <v>1.2999999523162842</v>
       </c>
       <c r="B7">
-        <v>-2.1511234081117436E-5</v>
+        <v>-1.2618587286183924E-9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2.7999999523162842</v>
+        <v>1.3999999761581421</v>
       </c>
       <c r="B8">
-        <v>-3.3885364246089011E-5</v>
+        <v>-1.6206509911853573E-8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3.0999999046325684</v>
+        <v>1.5</v>
       </c>
       <c r="B9">
-        <v>-4.831904880120419E-5</v>
+        <v>-1.3410327426299773E-7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3.4000000953674316</v>
+        <v>1.6000000238418579</v>
       </c>
       <c r="B10">
-        <v>-6.4483749156352133E-5</v>
+        <v>-5.7786155593930744E-7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3.7000000476837158</v>
+        <v>1.7000000476837158</v>
       </c>
       <c r="B11">
-        <v>-8.2087237387895584E-5</v>
+        <v>-1.4617525039284374E-6</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
+        <v>1.7999999523162842</v>
+      </c>
+      <c r="B12">
+        <v>-2.7578666959016118E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1.8999999761581421</v>
+      </c>
+      <c r="B13">
+        <v>-4.4340358726913109E-6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>-6.4706578086770605E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2.0999999046325684</v>
+      </c>
+      <c r="B15">
+        <v>-8.8516626419732347E-6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2.2000000476837158</v>
+      </c>
+      <c r="B16">
+        <v>-1.156148937297985E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2.2999999523162842</v>
+      </c>
+      <c r="B17">
+        <v>-1.4584730706701521E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2.4000000953674316</v>
+      </c>
+      <c r="B18">
+        <v>-1.7906242646859027E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2.5</v>
+      </c>
+      <c r="B19">
+        <v>-2.1511234081117436E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2.5999999046325684</v>
+      </c>
+      <c r="B20">
+        <v>-2.5385317712789401E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2.7000000476837158</v>
+      </c>
+      <c r="B21">
+        <v>-2.9514534617192112E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2.7999999523162842</v>
+      </c>
+      <c r="B22">
+        <v>-3.3885364246089011E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2.9000000953674316</v>
+      </c>
+      <c r="B23">
+        <v>-3.8484729884658009E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>-4.3300013203406706E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>3.0999999046325684</v>
+      </c>
+      <c r="B25">
+        <v>-4.831904880120419E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3.2000000476837158</v>
+      </c>
+      <c r="B26">
+        <v>-5.3530115110334009E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B27">
+        <v>-5.8921956224367023E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3.4000000953674316</v>
+      </c>
+      <c r="B28">
+        <v>-6.4483749156352133E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>3.5</v>
+      </c>
+      <c r="B29">
+        <v>-7.0205118390731514E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3.5999999046325684</v>
+      </c>
+      <c r="B30">
+        <v>-7.6076117693446577E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>3.7000000476837158</v>
+      </c>
+      <c r="B31">
+        <v>-8.2087237387895584E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>3.7999999523162842</v>
+      </c>
+      <c r="B32">
+        <v>-8.8229375251103193E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>3.9000000953674316</v>
+      </c>
+      <c r="B33">
+        <v>-9.4493836513720453E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>4</v>
       </c>
+      <c r="B34">
+        <v>-1.008723265840672E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFF7CF90-CF1B-4563-9AA1-D0FFD84A7A9F}">
+  <dimension ref="A1:B33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0.75</v>
+      </c>
+      <c r="B1">
+        <v>-1.0035839347055653E-12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.85000002384185791</v>
+      </c>
+      <c r="B2">
+        <v>-1.0760651267607835E-12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.94999998807907104</v>
+      </c>
+      <c r="B3">
+        <v>-2.610545677197984E-12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1.0499999523162842</v>
+      </c>
+      <c r="B4">
+        <v>-3.4787565189597913E-11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1.1500000953674316</v>
+      </c>
+      <c r="B5">
+        <v>-6.8250682883075342E-10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1.25</v>
+      </c>
+      <c r="B6">
+        <v>-1.1889514262009016E-8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1.3499999046325684</v>
+      </c>
+      <c r="B7">
+        <v>-1.4944647830361646E-7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1.4500000476837158</v>
+      </c>
+      <c r="B8">
+        <v>-1.178967295345501E-6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1.5499999523162842</v>
+      </c>
+      <c r="B9">
+        <v>-4.4375815377861727E-6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1.6500000953674316</v>
+      </c>
+      <c r="B10">
+        <v>-8.8389069787808694E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1.75</v>
+      </c>
+      <c r="B11">
+        <v>-1.2961154425283894E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1.8499999046325684</v>
+      </c>
       <c r="B12">
-        <v>-1.008723265840672E-4</v>
+        <v>-1.6761687220423482E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1.9500000476837158</v>
+      </c>
+      <c r="B13">
+        <v>-2.0366214812383987E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2.0499999523162842</v>
+      </c>
+      <c r="B14">
+        <v>-2.3810071070329286E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2.1500000953674316</v>
+      </c>
+      <c r="B15">
+        <v>-2.7098229111288674E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2.25</v>
+      </c>
+      <c r="B16">
+        <v>-3.0232442441047169E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2.3499999046325684</v>
+      </c>
+      <c r="B17">
+        <v>-3.321507028886117E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2.4500000476837158</v>
+      </c>
+      <c r="B18">
+        <v>-3.6049947084393352E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2.5499999523162842</v>
+      </c>
+      <c r="B19">
+        <v>-3.8740872696507722E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2.6500000953674316</v>
+      </c>
+      <c r="B20">
+        <v>-4.1292110836366192E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2.75</v>
+      </c>
+      <c r="B21">
+        <v>-4.3708336306735873E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2.8499999046325684</v>
+      </c>
+      <c r="B22">
+        <v>-4.5993590902071446E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2.9500000476837158</v>
+      </c>
+      <c r="B23">
+        <v>-4.8152880481211469E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3.0499999523162842</v>
+      </c>
+      <c r="B24">
+        <v>-5.0190403271699324E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>3.1500000953674316</v>
+      </c>
+      <c r="B25">
+        <v>-5.2110590331722051E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3.25</v>
+      </c>
+      <c r="B26">
+        <v>-5.3918462072033435E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>3.3499999046325684</v>
+      </c>
+      <c r="B27">
+        <v>-5.5617849284317344E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3.4500000476837158</v>
+      </c>
+      <c r="B28">
+        <v>-5.7213746913475916E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>3.5499999523162842</v>
+      </c>
+      <c r="B29">
+        <v>-5.8710047596832737E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3.6500000953674316</v>
+      </c>
+      <c r="B30">
+        <v>-6.0111109632998705E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>3.75</v>
+      </c>
+      <c r="B31">
+        <v>-6.1421436839736998E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>3.8499999046325684</v>
+      </c>
+      <c r="B32">
+        <v>-6.2644525314681232E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>3.9500000476837158</v>
+      </c>
+      <c r="B33">
+        <v>-6.3784958911128342E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2FA402-CE7F-4C63-B609-C30B0602857E}">
+  <dimension ref="A1:B34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B1">
+        <v>-3.3100189256174417E-12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B2">
+        <v>-3.3103979626969426E-12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B3">
+        <v>-3.3184017599746651E-12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B4">
+        <v>-3.487072392990842E-12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B5">
+        <v>-7.0098796559059373E-12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B6">
+        <v>-7.7762761507838007E-11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B7">
+        <v>-1.3068156556883537E-9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B8">
+        <v>-1.669910076884662E-8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B9">
+        <v>-1.3774010199085751E-7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B10">
+        <v>-5.9198924873271608E-7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B11">
+        <v>-1.4946666624382487E-6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B12">
+        <v>-2.815684865709045E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B13">
+        <v>-4.5207980292616412E-6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B14">
+        <v>-6.5886451920960099E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B15">
+        <v>-9.0014946181327105E-6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B16">
+        <v>-1.1742150491045322E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B17">
+        <v>-1.4793590707995463E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B18">
+        <v>-1.8139075109502301E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B19">
+        <v>-2.1762232790933922E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B20">
+        <v>-2.5647110305726528E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B21">
+        <v>-2.977818985527847E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B22">
+        <v>-3.4140397474402562E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B23">
+        <v>-3.87191103072837E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B24">
+        <v>-4.3500142055563629E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B25">
+        <v>-4.8469759349245578E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B26">
+        <v>-5.3614654461853206E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B27">
+        <v>-5.8921956224367023E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B28">
+        <v>-6.4379193645436317E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B29">
+        <v>-6.9974317739252001E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B30">
+        <v>-7.5695643317885697E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B31">
+        <v>-8.1531878095120192E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B32">
+        <v>-8.7472064478788525E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B33">
+        <v>-9.3505579570773989E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="B34">
+        <v>-9.9622113339137286E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>